<commit_message>
R2 hesaplama ve algoritmaların karşılaştırılması
</commit_message>
<xml_diff>
--- a/Prediction-MetotlarınKıyaslanması/veriler.xlsx
+++ b/Prediction-MetotlarınKıyaslanması/veriler.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eceha\Desktop\softbreak-ai-lab\Prediction-MetotlarınKıyaslanması\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093A8AD5-AC14-4036-9B19-49078CCDBDA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD201161-1DEA-4A2A-9166-BEFAFA1A6E92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{0063458B-E1C6-4A45-A4D4-80F751DCDCF2}"/>
   </bookViews>
   <sheets>
     <sheet name="veriler" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>boy</t>
   </si>
@@ -32,6 +45,9 @@
   </si>
   <si>
     <t>tahmin</t>
+  </si>
+  <si>
+    <t>başarı</t>
   </si>
 </sst>
 </file>
@@ -591,6 +607,1040 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="tr-TR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="tr-TR"/>
+              <a:t>Tahmin</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="tr-TR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="38100" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>veriler!$C$2:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>42</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>veriler!$D$2:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="22"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>44</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B6F7-4669-9E31-D67C33105075}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1442925408"/>
+        <c:axId val="1155533232"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1442925408"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1155533232"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1155533232"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="tr-TR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1442925408"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="tr-TR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>90792</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160252</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>397388</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>113300</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Grafik 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{79AA43BD-528D-5434-11E1-54AD955F4012}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -910,15 +1960,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AB2C03D-D51F-4672-801B-E30A60BD8320}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" zoomScale="153" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -931,8 +1981,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>130</v>
       </c>
@@ -942,8 +1995,18 @@
       <c r="C2">
         <v>10</v>
       </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <f>(C2-D2)*(C2-D2)</f>
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>125</v>
       </c>
@@ -953,8 +2016,18 @@
       <c r="C3">
         <v>11</v>
       </c>
+      <c r="D3">
+        <v>11</v>
+      </c>
+      <c r="E3">
+        <v>11</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F23" si="0">(C3-D3)*(C3-D3)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>135</v>
       </c>
@@ -964,8 +2037,18 @@
       <c r="C4">
         <v>10</v>
       </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>133</v>
       </c>
@@ -975,8 +2058,18 @@
       <c r="C5">
         <v>9</v>
       </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>129</v>
       </c>
@@ -986,8 +2079,18 @@
       <c r="C6">
         <v>12</v>
       </c>
+      <c r="D6">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>180</v>
       </c>
@@ -997,8 +2100,18 @@
       <c r="C7">
         <v>30</v>
       </c>
+      <c r="D7">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>190</v>
       </c>
@@ -1008,8 +2121,18 @@
       <c r="C8">
         <v>25</v>
       </c>
+      <c r="D8">
+        <v>26</v>
+      </c>
+      <c r="E8">
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>175</v>
       </c>
@@ -1019,8 +2142,18 @@
       <c r="C9">
         <v>35</v>
       </c>
+      <c r="D9">
+        <v>47</v>
+      </c>
+      <c r="E9">
+        <v>35</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>177</v>
       </c>
@@ -1030,8 +2163,18 @@
       <c r="C10">
         <v>22</v>
       </c>
+      <c r="D10">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>22</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>185</v>
       </c>
@@ -1041,8 +2184,18 @@
       <c r="C11">
         <v>33</v>
       </c>
+      <c r="D11">
+        <v>33</v>
+      </c>
+      <c r="E11">
+        <v>33</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>165</v>
       </c>
@@ -1052,8 +2205,18 @@
       <c r="C12">
         <v>27</v>
       </c>
+      <c r="D12">
+        <v>27</v>
+      </c>
+      <c r="E12">
+        <v>27</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>155</v>
       </c>
@@ -1063,8 +2226,18 @@
       <c r="C13">
         <v>44</v>
       </c>
+      <c r="D13">
+        <v>44</v>
+      </c>
+      <c r="E13">
+        <v>44</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>160</v>
       </c>
@@ -1074,8 +2247,18 @@
       <c r="C14">
         <v>39</v>
       </c>
+      <c r="D14">
+        <v>27</v>
+      </c>
+      <c r="E14">
+        <v>39</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>144</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>162</v>
       </c>
@@ -1085,8 +2268,18 @@
       <c r="C15">
         <v>41</v>
       </c>
+      <c r="D15">
+        <v>40</v>
+      </c>
+      <c r="E15">
+        <v>41</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>167</v>
       </c>
@@ -1096,8 +2289,18 @@
       <c r="C16">
         <v>55</v>
       </c>
+      <c r="D16">
+        <v>50</v>
+      </c>
+      <c r="E16">
+        <v>55</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>174</v>
       </c>
@@ -1107,8 +2310,18 @@
       <c r="C17">
         <v>47</v>
       </c>
+      <c r="D17">
+        <v>47</v>
+      </c>
+      <c r="E17">
+        <v>47</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>193</v>
       </c>
@@ -1118,8 +2331,18 @@
       <c r="C18">
         <v>23</v>
       </c>
+      <c r="D18">
+        <v>29</v>
+      </c>
+      <c r="E18">
+        <v>23</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>187</v>
       </c>
@@ -1129,8 +2352,18 @@
       <c r="C19">
         <v>27</v>
       </c>
+      <c r="D19">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>27</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>183</v>
       </c>
@@ -1140,8 +2373,18 @@
       <c r="C20">
         <v>28</v>
       </c>
+      <c r="D20">
+        <v>33</v>
+      </c>
+      <c r="E20">
+        <v>28</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>159</v>
       </c>
@@ -1151,8 +2394,18 @@
       <c r="C21">
         <v>29</v>
       </c>
+      <c r="D21">
+        <v>22</v>
+      </c>
+      <c r="E21">
+        <v>29</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>164</v>
       </c>
@@ -1162,8 +2415,18 @@
       <c r="C22">
         <v>32</v>
       </c>
+      <c r="D22">
+        <v>33</v>
+      </c>
+      <c r="E22">
+        <v>32</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>166</v>
       </c>
@@ -1172,9 +2435,26 @@
       </c>
       <c r="C23">
         <v>42</v>
+      </c>
+      <c r="D23">
+        <v>44</v>
+      </c>
+      <c r="E23">
+        <v>42</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D24">
+        <f>AVERAGE(D2:D23)</f>
+        <v>28.863636363636363</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>